<commit_message>
done with the designs
</commit_message>
<xml_diff>
--- a/ALA.xlsx
+++ b/ALA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalve\Documents\GitHub\BLG222\BLG222\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cakirv\Documents\GitHub\BLG222\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEE150F-0495-4C40-8001-417292D8D2D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22063401-C088-4B1B-8EF7-BCABEBF3A4F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{DB7D6FC1-A308-4B50-87C6-D2818FA8AF32}"/>
+    <workbookView xWindow="-40965" yWindow="675" windowWidth="21600" windowHeight="11370" xr2:uid="{DB7D6FC1-A308-4B50-87C6-D2818FA8AF32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="255">
   <si>
     <t>RX &lt;-- IROUT(0-7)</t>
   </si>
@@ -628,6 +628,174 @@
   </si>
   <si>
     <t>PASSALUARF</t>
+  </si>
+  <si>
+    <t>ENMUXA</t>
+  </si>
+  <si>
+    <t>ENMUXB</t>
+  </si>
+  <si>
+    <t>ENMUXC</t>
+  </si>
+  <si>
+    <t>140000</t>
+  </si>
+  <si>
+    <t>145050</t>
+  </si>
+  <si>
+    <t>146000</t>
+  </si>
+  <si>
+    <t>168E01</t>
+  </si>
+  <si>
+    <t>0001E0</t>
+  </si>
+  <si>
+    <t>028000</t>
+  </si>
+  <si>
+    <t>028E01</t>
+  </si>
+  <si>
+    <t>000061</t>
+  </si>
+  <si>
+    <t>038000</t>
+  </si>
+  <si>
+    <t>030000</t>
+  </si>
+  <si>
+    <t>147184</t>
+  </si>
+  <si>
+    <t>147004</t>
+  </si>
+  <si>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>028E04</t>
+  </si>
+  <si>
+    <t>028F84</t>
+  </si>
+  <si>
+    <t>147186</t>
+  </si>
+  <si>
+    <t>028186</t>
+  </si>
+  <si>
+    <t>147006</t>
+  </si>
+  <si>
+    <t>028006</t>
+  </si>
+  <si>
+    <t>147187</t>
+  </si>
+  <si>
+    <t>028F87</t>
+  </si>
+  <si>
+    <t>147007</t>
+  </si>
+  <si>
+    <t>028E07</t>
+  </si>
+  <si>
+    <t>147188</t>
+  </si>
+  <si>
+    <t>028F88</t>
+  </si>
+  <si>
+    <t>147008</t>
+  </si>
+  <si>
+    <t>028E08</t>
+  </si>
+  <si>
+    <t>1C00050</t>
+  </si>
+  <si>
+    <t>1E00050</t>
+  </si>
+  <si>
+    <t>0030000</t>
+  </si>
+  <si>
+    <t>0180000</t>
+  </si>
+  <si>
+    <t>01C0000</t>
+  </si>
+  <si>
+    <t>0038000</t>
+  </si>
+  <si>
+    <t>0000180</t>
+  </si>
+  <si>
+    <t>0000000</t>
+  </si>
+  <si>
+    <t>0028C50</t>
+  </si>
+  <si>
+    <t>0000060</t>
+  </si>
+  <si>
+    <t>0028A00</t>
+  </si>
+  <si>
+    <t>0028E0B</t>
+  </si>
+  <si>
+    <t>014700B</t>
+  </si>
+  <si>
+    <t>002F18B</t>
+  </si>
+  <si>
+    <t>0028E0A</t>
+  </si>
+  <si>
+    <t>014700A</t>
+  </si>
+  <si>
+    <t>0028F8A</t>
+  </si>
+  <si>
+    <t>014718A</t>
+  </si>
+  <si>
+    <t>0028E02</t>
+  </si>
+  <si>
+    <t>0147002</t>
+  </si>
+  <si>
+    <t>0030F82</t>
+  </si>
+  <si>
+    <t>0147182</t>
+  </si>
+  <si>
+    <t>0028E08</t>
+  </si>
+  <si>
+    <t>0147008</t>
+  </si>
+  <si>
+    <t>0028E07</t>
+  </si>
+  <si>
+    <t>0147007</t>
   </si>
 </sst>
 </file>
@@ -682,11 +850,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +875,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1001,12 +1171,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F692F4-DF4D-4179-A8A6-7B3A696DFCB2}">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomLeft" activeCell="V55" sqref="V55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,16 +1190,22 @@
     <col min="7" max="7" width="6.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="7" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="11" width="9.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="1"/>
+    <col min="21" max="21" width="31" style="5" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>189</v>
       </c>
@@ -1058,29 +1234,38 @@
         <v>115</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="R1" s="3"/>
-    </row>
-    <row r="2" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1297,7 @@
         <v>123</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>123</v>
@@ -1121,7 +1306,7 @@
         <v>125</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>125</v>
@@ -1130,10 +1315,26 @@
         <v>125</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U2" s="5" t="str">
+        <f>D2&amp;E2&amp;F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2&amp;S2&amp;T2</f>
+        <v>0000101000000000000000000</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1165,28 +1366,44 @@
         <v>123</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M3" s="1" t="s">
         <v>125</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>125</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U3" s="5" t="str">
+        <f t="shared" ref="U3:U58" si="0">D3&amp;E3&amp;F3&amp;G3&amp;H3&amp;I3&amp;J3&amp;K3&amp;L3&amp;M3&amp;N3&amp;O3&amp;P3&amp;Q3&amp;R3&amp;S3&amp;T3</f>
+        <v>0000101000101000001010000</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1218,28 +1435,44 @@
         <v>123</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>123</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>127</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U4" s="5" t="str">
+        <f>D4&amp;E4&amp;F4&amp;G4&amp;H4&amp;I4&amp;J4&amp;K4&amp;L4&amp;M4&amp;N4&amp;O4&amp;P4&amp;Q4&amp;R4&amp;S4&amp;T4</f>
+        <v>0000000000000000111100000</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1271,16 +1504,16 @@
         <v>124</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
+      <c r="M5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
@@ -1288,11 +1521,27 @@
       <c r="P5" s="1">
         <v>0</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U5" s="5" t="str">
+        <f>D5&amp;E5&amp;F5&amp;G5&amp;H5&amp;I5&amp;J5&amp;K5&amp;L5&amp;M5&amp;N5&amp;O5&amp;P5&amp;Q5&amp;R5&amp;S5&amp;T5</f>
+        <v>0000000101000000000000000</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1324,16 +1573,16 @@
         <v>123</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
+      <c r="M6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O6" s="1">
         <v>0</v>
@@ -1341,11 +1590,27 @@
       <c r="P6" s="1">
         <v>0</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000110000000000000</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1377,28 +1642,44 @@
         <v>124</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
       <c r="O7" s="1">
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">0000000101000111000000001 </v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1430,28 +1711,44 @@
         <v>124</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U8" s="5" t="str">
+        <f>D8&amp;E8&amp;F8&amp;G8&amp;H8&amp;I8&amp;J8&amp;K8&amp;L8&amp;M8&amp;N8&amp;O8&amp;P8&amp;Q8&amp;R8&amp;S8&amp;T8</f>
+        <v>0000101101000111000000001</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1483,28 +1780,44 @@
         <v>123</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="1">
-        <v>0</v>
+      <c r="M9" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
       </c>
       <c r="Q9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U9" s="5" t="str">
+        <f>D9&amp;E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9&amp;O9&amp;P9&amp;Q9&amp;R9&amp;S9&amp;T9</f>
+        <v>0000000000000000001100001</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1536,28 +1849,44 @@
         <v>123</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0</v>
+      <c r="M10" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O10" s="1">
         <v>0</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>127</v>
+      <c r="P10" s="1">
+        <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U10" s="5" t="str">
+        <f>D10&amp;E10&amp;F10&amp;G10&amp;H10&amp;I10&amp;J10&amp;K10&amp;L10&amp;M10&amp;N10&amp;O10&amp;P10&amp;Q10&amp;R10&amp;S10&amp;T10</f>
+        <v>0000101000101000001010000</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1589,16 +1918,16 @@
         <v>137</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>0</v>
+      <c r="M11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O11" s="1">
         <v>0</v>
@@ -1606,11 +1935,27 @@
       <c r="P11" s="1">
         <v>0</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U11" s="5" t="str">
+        <f>D11&amp;E11&amp;F11&amp;G11&amp;H11&amp;I11&amp;J11&amp;K11&amp;L11&amp;M11&amp;N11&amp;O11&amp;P11&amp;Q11&amp;R11&amp;S11&amp;T11</f>
+        <v>0000000111000000000000000</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1642,16 +1987,16 @@
         <v>136</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
+      <c r="M12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O12" s="1">
         <v>0</v>
@@ -1659,11 +2004,27 @@
       <c r="P12" s="1">
         <v>0</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000110000000000000000</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1695,28 +2056,44 @@
         <v>123</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M13" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U13" s="5" t="str">
+        <f>D13&amp;E13&amp;F13&amp;G13&amp;H13&amp;I13&amp;J13&amp;K13&amp;L13&amp;M13&amp;N13&amp;O13&amp;P13&amp;Q13&amp;R13&amp;S13&amp;T13</f>
+        <v>0000101000111000110000100</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1748,16 +2125,16 @@
         <v>123</v>
       </c>
       <c r="K14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
+      <c r="M14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O14" s="1">
         <v>0</v>
@@ -1765,11 +2142,27 @@
       <c r="P14" s="1">
         <v>0</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U14" s="5" t="str">
+        <f>D14&amp;E14&amp;F14&amp;G14&amp;H14&amp;I14&amp;J14&amp;K14&amp;L14&amp;M14&amp;N14&amp;O14&amp;P14&amp;Q14&amp;R14&amp;S14&amp;T14</f>
+        <v>0000101000111000000000100</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1801,28 +2194,44 @@
         <v>123</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1" t="s">
+      <c r="N15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U15" s="5" t="str">
+        <f>D15&amp;E15&amp;F15&amp;G15&amp;H15&amp;I15&amp;J15&amp;K15&amp;L15&amp;M15&amp;N15&amp;O15&amp;P15&amp;Q15&amp;R15&amp;S15&amp;T15</f>
+        <v>0000101000111000000000100</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1854,28 +2263,44 @@
         <v>124</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1" t="s">
+      <c r="O16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000111110000100</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1907,28 +2332,44 @@
         <v>124</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M17" s="1">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1">
-        <v>0</v>
-      </c>
       <c r="O17" s="1">
         <v>0</v>
       </c>
       <c r="P17" s="1">
         <v>0</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000111000000100</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1960,7 +2401,7 @@
         <v>123</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>123</v>
@@ -1968,20 +2409,36 @@
       <c r="M18" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="N18" s="1">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1">
-        <v>0</v>
-      </c>
-      <c r="P18" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="1" t="s">
+      <c r="N18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000000000000000000100</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2013,28 +2470,44 @@
         <v>123</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M19" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N19" s="1">
-        <v>0</v>
-      </c>
-      <c r="O19" s="1">
-        <v>0</v>
-      </c>
-      <c r="P19" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000110000110</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2066,28 +2539,44 @@
         <v>124</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>123</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N20" s="1">
-        <v>0</v>
-      </c>
-      <c r="O20" s="1">
-        <v>0</v>
-      </c>
-      <c r="P20" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000000110000110</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -2119,16 +2608,16 @@
         <v>123</v>
       </c>
       <c r="K21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M21" s="1">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1">
-        <v>0</v>
+      <c r="M21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O21" s="1">
         <v>0</v>
@@ -2136,11 +2625,27 @@
       <c r="P21" s="1">
         <v>0</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000000000110</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
@@ -2172,16 +2677,16 @@
         <v>124</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M22" s="1">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
+      <c r="M22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O22" s="1">
         <v>0</v>
@@ -2189,11 +2694,27 @@
       <c r="P22" s="1">
         <v>0</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U22" s="5" t="str">
+        <f>D22&amp;E22&amp;F22&amp;G22&amp;H22&amp;I22&amp;J22&amp;K22&amp;L22&amp;M22&amp;N22&amp;O22&amp;P22&amp;Q22&amp;R22&amp;S22&amp;T22</f>
+        <v>0000000101000000000000110</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2225,28 +2746,44 @@
         <v>123</v>
       </c>
       <c r="K23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <v>0</v>
-      </c>
-      <c r="P23" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U23" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000110000111</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -2278,28 +2815,44 @@
         <v>124</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="1" t="s">
+      <c r="O24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U24" s="5" t="str">
+        <f>D24&amp;E24&amp;F24&amp;G24&amp;H24&amp;I24&amp;J24&amp;K24&amp;L24&amp;M24&amp;N24&amp;O24&amp;P24&amp;Q24&amp;R24&amp;S24&amp;T24</f>
+        <v>0000000101000111110000111</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2331,16 +2884,16 @@
         <v>123</v>
       </c>
       <c r="K25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M25" s="1">
-        <v>0</v>
-      </c>
-      <c r="N25" s="1">
-        <v>0</v>
+      <c r="M25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
@@ -2348,11 +2901,27 @@
       <c r="P25" s="1">
         <v>0</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" s="1">
+        <v>0</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U25" s="5" t="str">
+        <f>D25&amp;E25&amp;F25&amp;G25&amp;H25&amp;I25&amp;J25&amp;K25&amp;L25&amp;M25&amp;N25&amp;O25&amp;P25&amp;Q25&amp;R25&amp;S25&amp;T25</f>
+        <v>0000101000111000000000111</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -2384,28 +2953,44 @@
         <v>124</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M26" s="1">
-        <v>0</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
       <c r="O26" s="1">
         <v>0</v>
       </c>
       <c r="P26" s="1">
         <v>0</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" s="1">
+        <v>0</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U26" s="5" t="str">
+        <f>D26&amp;E26&amp;F26&amp;G26&amp;H26&amp;I26&amp;J26&amp;K26&amp;L26&amp;M26&amp;N26&amp;O26&amp;P26&amp;Q26&amp;R26&amp;S26&amp;T26</f>
+        <v>0000000101000111000000111</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2437,16 +3022,16 @@
         <v>123</v>
       </c>
       <c r="K27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M27" s="1">
-        <v>0</v>
-      </c>
-      <c r="N27" s="1">
-        <v>0</v>
+      <c r="M27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O27" s="1">
         <v>0</v>
@@ -2454,11 +3039,27 @@
       <c r="P27" s="1">
         <v>0</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" s="1">
+        <v>0</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0</v>
+      </c>
+      <c r="T27" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U27" s="5" t="str">
+        <f>D27&amp;E27&amp;F27&amp;G27&amp;H27&amp;I27&amp;J27&amp;K27&amp;L27&amp;M27&amp;N27&amp;O27&amp;P27&amp;Q27&amp;R27&amp;S27&amp;T27</f>
+        <v>0000101000111000000000111</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -2490,28 +3091,44 @@
         <v>124</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L28" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M28" s="1">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
       <c r="O28" s="1">
         <v>0</v>
       </c>
       <c r="P28" s="1">
         <v>0</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U28" s="5" t="str">
+        <f>D28&amp;E28&amp;F28&amp;G28&amp;H28&amp;I28&amp;J28&amp;K28&amp;L28&amp;M28&amp;N28&amp;O28&amp;P28&amp;Q28&amp;R28&amp;S28&amp;T28</f>
+        <v>0000000101000111000000111</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2543,28 +3160,44 @@
         <v>123</v>
       </c>
       <c r="K29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M29" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N29" s="1">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U29" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000110001000</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
@@ -2596,28 +3229,44 @@
         <v>124</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N30" s="1">
-        <v>0</v>
-      </c>
-      <c r="O30" s="1">
-        <v>0</v>
-      </c>
-      <c r="P30" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="1" t="s">
+      <c r="O30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U30" s="5" t="str">
+        <f>D30&amp;E30&amp;F30&amp;G30&amp;H30&amp;I30&amp;J30&amp;K30&amp;L30&amp;M30&amp;N30&amp;O30&amp;P30&amp;Q30&amp;R30&amp;S30&amp;T30</f>
+        <v>0000000101000111110001000</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -2649,16 +3298,16 @@
         <v>123</v>
       </c>
       <c r="K31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M31" s="1">
-        <v>0</v>
-      </c>
-      <c r="N31" s="1">
-        <v>0</v>
+      <c r="M31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O31" s="1">
         <v>0</v>
@@ -2666,11 +3315,27 @@
       <c r="P31" s="1">
         <v>0</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="Q31" s="1">
+        <v>0</v>
+      </c>
+      <c r="R31" s="1">
+        <v>0</v>
+      </c>
+      <c r="S31" s="1">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U31" s="5" t="str">
+        <f>D31&amp;E31&amp;F31&amp;G31&amp;H31&amp;I31&amp;J31&amp;K31&amp;L31&amp;M31&amp;N31&amp;O31&amp;P31&amp;Q31&amp;R31&amp;S31&amp;T31</f>
+        <v>0000101000111000000001000</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -2702,28 +3367,44 @@
         <v>124</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M32" s="1">
-        <v>0</v>
-      </c>
-      <c r="N32" s="1">
-        <v>0</v>
-      </c>
       <c r="O32" s="1">
         <v>0</v>
       </c>
       <c r="P32" s="1">
         <v>0</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" s="1">
+        <v>0</v>
+      </c>
+      <c r="R32" s="1">
+        <v>0</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0</v>
+      </c>
+      <c r="T32" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U32" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000111000001000</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -2755,16 +3436,16 @@
         <v>123</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M33" s="1">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1">
-        <v>0</v>
+      <c r="M33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O33" s="1">
         <v>0</v>
@@ -2772,11 +3453,27 @@
       <c r="P33" s="1">
         <v>0</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="Q33" s="1">
+        <v>0</v>
+      </c>
+      <c r="R33" s="1">
+        <v>0</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000000001000</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -2808,28 +3505,44 @@
         <v>124</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M34" s="1">
-        <v>0</v>
-      </c>
-      <c r="N34" s="1">
-        <v>0</v>
-      </c>
       <c r="O34" s="1">
         <v>0</v>
       </c>
       <c r="P34" s="1">
         <v>0</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="Q34" s="1">
+        <v>0</v>
+      </c>
+      <c r="R34" s="1">
+        <v>0</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0</v>
+      </c>
+      <c r="T34" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U34" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000111000001000</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -2861,28 +3574,44 @@
         <v>123</v>
       </c>
       <c r="K35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M35" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N35" s="1">
-        <v>0</v>
-      </c>
-      <c r="O35" s="1">
-        <v>0</v>
-      </c>
-      <c r="P35" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U35" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000110000010</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -2914,28 +3643,44 @@
         <v>136</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N36" s="1">
-        <v>0</v>
-      </c>
-      <c r="O36" s="1">
-        <v>0</v>
-      </c>
-      <c r="P36" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="1" t="s">
+      <c r="O36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U36" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000110000111110000010</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -2967,16 +3712,16 @@
         <v>123</v>
       </c>
       <c r="K37" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M37" s="1">
-        <v>0</v>
-      </c>
-      <c r="N37" s="1">
-        <v>0</v>
+      <c r="M37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O37" s="1">
         <v>0</v>
@@ -2984,11 +3729,27 @@
       <c r="P37" s="1">
         <v>0</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U37" s="5" t="str">
+        <f>D37&amp;E37&amp;F37&amp;G37&amp;H37&amp;I37&amp;J37&amp;K37&amp;L37&amp;M37&amp;N37&amp;O37&amp;P37&amp;Q37&amp;R37&amp;S37&amp;T37</f>
+        <v>0000101000111000000000010</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -3020,28 +3781,44 @@
         <v>124</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N38" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M38" s="1">
-        <v>0</v>
-      </c>
-      <c r="N38" s="1">
-        <v>0</v>
-      </c>
       <c r="O38" s="1">
         <v>0</v>
       </c>
       <c r="P38" s="1">
         <v>0</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="Q38" s="1">
+        <v>0</v>
+      </c>
+      <c r="R38" s="1">
+        <v>0</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U38" s="5" t="str">
+        <f>D38&amp;E38&amp;F38&amp;G38&amp;H38&amp;I38&amp;J38&amp;K38&amp;L38&amp;M38&amp;N38&amp;O38&amp;P38&amp;Q38&amp;R38&amp;S38&amp;T38</f>
+        <v>0000000101000111000000010</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -3073,28 +3850,44 @@
         <v>123</v>
       </c>
       <c r="K39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M39" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N39" s="1">
-        <v>0</v>
-      </c>
-      <c r="O39" s="1">
-        <v>0</v>
-      </c>
-      <c r="P39" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="R39" s="1">
+        <v>0</v>
+      </c>
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U39" s="5" t="str">
+        <f>D39&amp;E39&amp;F39&amp;G39&amp;H39&amp;I39&amp;J39&amp;K39&amp;L39&amp;M39&amp;N39&amp;O39&amp;P39&amp;Q39&amp;R39&amp;S39&amp;T39</f>
+        <v>0000101000111000110001010</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -3126,28 +3919,44 @@
         <v>124</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L40" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N40" s="1">
-        <v>0</v>
-      </c>
-      <c r="O40" s="1">
-        <v>0</v>
-      </c>
-      <c r="P40" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="1" t="s">
+      <c r="O40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="R40" s="1">
+        <v>0</v>
+      </c>
+      <c r="S40" s="1">
+        <v>0</v>
+      </c>
+      <c r="T40" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U40" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000111110001010</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
@@ -3179,16 +3988,16 @@
         <v>123</v>
       </c>
       <c r="K41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M41" s="1">
-        <v>0</v>
-      </c>
-      <c r="N41" s="1">
-        <v>0</v>
+      <c r="M41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O41" s="1">
         <v>0</v>
@@ -3196,11 +4005,27 @@
       <c r="P41" s="1">
         <v>0</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0</v>
+      </c>
+      <c r="S41" s="1">
+        <v>0</v>
+      </c>
+      <c r="T41" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U41" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000000001010</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
@@ -3232,28 +4057,44 @@
         <v>124</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M42" s="1">
-        <v>0</v>
-      </c>
-      <c r="N42" s="1">
-        <v>0</v>
-      </c>
       <c r="O42" s="1">
         <v>0</v>
       </c>
       <c r="P42" s="1">
         <v>0</v>
       </c>
-      <c r="Q42" s="1" t="s">
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <v>0</v>
+      </c>
+      <c r="T42" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U42" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000111000001010</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
@@ -3285,28 +4126,44 @@
         <v>124</v>
       </c>
       <c r="K43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="M43" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N43" s="1">
-        <v>0</v>
-      </c>
-      <c r="O43" s="1">
-        <v>0</v>
-      </c>
-      <c r="P43" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1">
+        <v>0</v>
+      </c>
+      <c r="S43" s="1">
+        <v>0</v>
+      </c>
+      <c r="T43" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U43" s="5" t="str">
+        <f>D43&amp;E43&amp;F43&amp;G43&amp;H43&amp;I43&amp;J43&amp;K43&amp;L43&amp;M43&amp;N43&amp;O43&amp;P43&amp;Q43&amp;R43&amp;S43&amp;T43</f>
+        <v>0000000101111000110001011</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
@@ -3338,28 +4195,44 @@
         <v>124</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N44" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M44" s="1">
-        <v>0</v>
-      </c>
-      <c r="N44" s="1">
-        <v>0</v>
-      </c>
       <c r="O44" s="1">
         <v>0</v>
       </c>
       <c r="P44" s="1">
         <v>0</v>
       </c>
-      <c r="Q44" s="1" t="s">
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0</v>
+      </c>
+      <c r="S44" s="1">
+        <v>0</v>
+      </c>
+      <c r="T44" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U44" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000111000001011</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -3391,16 +4264,16 @@
         <v>123</v>
       </c>
       <c r="K45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M45" s="1">
-        <v>0</v>
-      </c>
-      <c r="N45" s="1">
-        <v>0</v>
+      <c r="M45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O45" s="1">
         <v>0</v>
@@ -3408,11 +4281,27 @@
       <c r="P45" s="1">
         <v>0</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+      <c r="R45" s="1">
+        <v>0</v>
+      </c>
+      <c r="S45" s="1">
+        <v>0</v>
+      </c>
+      <c r="T45" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U45" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000101000111000000001011</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>28</v>
       </c>
@@ -3444,28 +4333,44 @@
         <v>124</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L46" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N46" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M46" s="1">
-        <v>0</v>
-      </c>
-      <c r="N46" s="1">
-        <v>0</v>
-      </c>
       <c r="O46" s="1">
         <v>0</v>
       </c>
       <c r="P46" s="1">
         <v>0</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="Q46" s="1">
+        <v>0</v>
+      </c>
+      <c r="R46" s="1">
+        <v>0</v>
+      </c>
+      <c r="S46" s="1">
+        <v>0</v>
+      </c>
+      <c r="T46" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U46" s="5" t="str">
+        <f>D46&amp;E46&amp;F46&amp;G46&amp;H46&amp;I46&amp;J46&amp;K46&amp;L46&amp;M46&amp;N46&amp;O46&amp;P46&amp;Q46&amp;R46&amp;S46&amp;T46</f>
+        <v>0000000101000111000001011</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
@@ -3497,28 +4402,44 @@
         <v>124</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N47" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M47" s="1">
-        <v>0</v>
-      </c>
-      <c r="N47" s="1">
-        <v>0</v>
-      </c>
       <c r="O47" s="1">
         <v>0</v>
       </c>
       <c r="P47" s="1">
         <v>0</v>
       </c>
-      <c r="Q47" s="1" t="s">
+      <c r="Q47" s="1">
+        <v>0</v>
+      </c>
+      <c r="R47" s="1">
+        <v>0</v>
+      </c>
+      <c r="S47" s="1">
+        <v>0</v>
+      </c>
+      <c r="T47" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U47" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000101000101000000000</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -3550,28 +4471,44 @@
         <v>123</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M48" s="1">
-        <v>0</v>
+      <c r="M48" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="O48" s="1">
+        <v>0</v>
       </c>
       <c r="P48" s="1">
         <v>0</v>
       </c>
       <c r="Q48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S48" s="1">
+        <v>0</v>
+      </c>
+      <c r="T48" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U48" s="5" t="str">
+        <f>D48&amp;E48&amp;F48&amp;G48&amp;H48&amp;I48&amp;J48&amp;K48&amp;L48&amp;M48&amp;N48&amp;O48&amp;P48&amp;Q48&amp;R48&amp;S48&amp;T48</f>
+        <v>0000000000000000001100000</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -3603,35 +4540,51 @@
         <v>124</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N49" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M49" s="1">
-        <v>0</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="O49" s="1">
         <v>0</v>
       </c>
-      <c r="P49" s="1" t="s">
-        <v>127</v>
+      <c r="P49" s="1">
+        <v>0</v>
       </c>
       <c r="Q49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R49" s="1">
+        <v>0</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T49" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U49" s="5" t="str">
+        <f>D49&amp;E49&amp;F49&amp;G49&amp;H49&amp;I49&amp;J49&amp;K49&amp;L49&amp;M49&amp;N49&amp;O49&amp;P49&amp;Q49&amp;R49&amp;S49&amp;T49</f>
+        <v>0000000101000110001010000</v>
+      </c>
+      <c r="V49" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>198</v>
       </c>
       <c r="D50" s="1">
@@ -3656,16 +4609,16 @@
         <v>123</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M50" s="1">
-        <v>0</v>
-      </c>
-      <c r="N50" s="1">
-        <v>0</v>
+      <c r="M50" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O50" s="1">
         <v>0</v>
@@ -3673,18 +4626,34 @@
       <c r="P50" s="1">
         <v>0</v>
       </c>
-      <c r="Q50" s="1" t="s">
+      <c r="Q50" s="1">
+        <v>0</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0</v>
+      </c>
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+      <c r="T50" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U50" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000000000000000000000</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>197</v>
       </c>
       <c r="D51" s="1">
@@ -3709,28 +4678,44 @@
         <v>123</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>123</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N51" s="1">
-        <v>0</v>
-      </c>
-      <c r="O51" s="1">
-        <v>0</v>
-      </c>
-      <c r="P51" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>0</v>
+      </c>
+      <c r="R51" s="1">
+        <v>0</v>
+      </c>
+      <c r="S51" s="1">
+        <v>0</v>
+      </c>
+      <c r="T51" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U51" s="5" t="str">
+        <f>D51&amp;E51&amp;F51&amp;G51&amp;H51&amp;I51&amp;J51&amp;K51&amp;L51&amp;M51&amp;N51&amp;O51&amp;P51&amp;Q51&amp;R51&amp;S51&amp;T51</f>
+        <v>0000000000000000110000000</v>
+      </c>
+      <c r="V51" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -3762,16 +4747,16 @@
         <v>137</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M52" s="1">
-        <v>0</v>
-      </c>
-      <c r="N52" s="1">
-        <v>0</v>
+      <c r="M52" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O52" s="1">
         <v>0</v>
@@ -3779,11 +4764,27 @@
       <c r="P52" s="1">
         <v>0</v>
       </c>
-      <c r="Q52" s="1" t="s">
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
+      <c r="R52" s="1">
+        <v>0</v>
+      </c>
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+      <c r="T52" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U52" s="5" t="str">
+        <f>D52&amp;E52&amp;F52&amp;G52&amp;H52&amp;I52&amp;J52&amp;K52&amp;L52&amp;M52&amp;N52&amp;O52&amp;P52&amp;Q52&amp;R52&amp;S52&amp;T52</f>
+        <v>0000000111000000000000000</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
@@ -3815,16 +4816,16 @@
         <v>123</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M53" s="1">
-        <v>0</v>
-      </c>
-      <c r="N53" s="1">
-        <v>0</v>
+      <c r="M53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O53" s="1">
         <v>0</v>
@@ -3832,11 +4833,27 @@
       <c r="P53" s="1">
         <v>0</v>
       </c>
-      <c r="Q53" s="1" t="s">
+      <c r="Q53" s="1">
+        <v>0</v>
+      </c>
+      <c r="R53" s="1">
+        <v>0</v>
+      </c>
+      <c r="S53" s="1">
+        <v>0</v>
+      </c>
+      <c r="T53" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U53" s="5" t="str">
+        <f>D53&amp;E53&amp;F53&amp;G53&amp;H53&amp;I53&amp;J53&amp;K53&amp;L53&amp;M53&amp;N53&amp;O53&amp;P53&amp;Q53&amp;R53&amp;S53&amp;T53</f>
+        <v>0000111000000000000000000</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -3868,16 +4885,16 @@
         <v>136</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M54" s="1">
-        <v>0</v>
-      </c>
-      <c r="N54" s="1">
-        <v>0</v>
+      <c r="M54" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O54" s="1">
         <v>0</v>
@@ -3885,11 +4902,27 @@
       <c r="P54" s="1">
         <v>0</v>
       </c>
-      <c r="Q54" s="1" t="s">
+      <c r="Q54" s="1">
+        <v>0</v>
+      </c>
+      <c r="R54" s="1">
+        <v>0</v>
+      </c>
+      <c r="S54" s="1">
+        <v>0</v>
+      </c>
+      <c r="T54" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U54" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000110000000000000000</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -3921,16 +4954,16 @@
         <v>123</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M55" s="1">
-        <v>0</v>
-      </c>
-      <c r="N55" s="1">
-        <v>0</v>
+      <c r="M55" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O55" s="1">
         <v>0</v>
@@ -3938,11 +4971,27 @@
       <c r="P55" s="1">
         <v>0</v>
       </c>
-      <c r="Q55" s="1" t="s">
+      <c r="Q55" s="1">
+        <v>0</v>
+      </c>
+      <c r="R55" s="1">
+        <v>0</v>
+      </c>
+      <c r="S55" s="1">
+        <v>0</v>
+      </c>
+      <c r="T55" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U55" s="5" t="str">
+        <f>D55&amp;E55&amp;F55&amp;G55&amp;H55&amp;I55&amp;J55&amp;K55&amp;L55&amp;M55&amp;N55&amp;O55&amp;P55&amp;Q55&amp;R55&amp;S55&amp;T55</f>
+        <v>0000110000000000000000000</v>
+      </c>
+      <c r="V55" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
@@ -3974,28 +5023,44 @@
         <v>123</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M56" s="1">
-        <v>0</v>
+      <c r="M56" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="O56" s="1">
+        <v>0</v>
+      </c>
+      <c r="P56" s="1">
+        <v>0</v>
       </c>
       <c r="Q56" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T56" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U56" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>1110000000000000001010000</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -4027,28 +5092,44 @@
         <v>123</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M57" s="1">
-        <v>0</v>
+      <c r="M57" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="O57" s="1">
+        <v>0</v>
+      </c>
+      <c r="P57" s="1">
+        <v>0</v>
       </c>
       <c r="Q57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T57" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U57" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>1111000000000000001010000</v>
+      </c>
+      <c r="V57" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
@@ -4080,16 +5161,16 @@
         <v>136</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M58" s="1">
-        <v>0</v>
-      </c>
-      <c r="N58" s="1">
-        <v>0</v>
+      <c r="M58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="O58" s="1">
         <v>0</v>
@@ -4097,8 +5178,24 @@
       <c r="P58" s="1">
         <v>0</v>
       </c>
-      <c r="Q58" s="1" t="s">
+      <c r="Q58" s="1">
+        <v>0</v>
+      </c>
+      <c r="R58" s="1">
+        <v>0</v>
+      </c>
+      <c r="S58" s="1">
+        <v>0</v>
+      </c>
+      <c r="T58" s="1" t="s">
         <v>126</v>
+      </c>
+      <c r="U58" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000110000000000000000</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I HOPE THIS THE LAST ONE
</commit_message>
<xml_diff>
--- a/ALA.xlsx
+++ b/ALA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cakirv\Documents\GitHub\BLG222\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE395DA3-893C-473C-9457-C6AAA0607965}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6701E78F-EC3A-4C6C-ABBB-375CA58E00AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB7D6FC1-A308-4B50-87C6-D2818FA8AF32}"/>
   </bookViews>
@@ -645,9 +645,6 @@
     <t>146000</t>
   </si>
   <si>
-    <t>168E01</t>
-  </si>
-  <si>
     <t>0001E0</t>
   </si>
   <si>
@@ -970,6 +967,9 @@
   </si>
   <si>
     <t>HEX</t>
+  </si>
+  <si>
+    <t>16FE01</t>
   </si>
 </sst>
 </file>
@@ -998,12 +998,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1018,13 +1024,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1344,13 +1351,13 @@
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomLeft" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
@@ -1434,7 +1441,7 @@
       </c>
       <c r="V1" s="3"/>
       <c r="W1" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1442,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>127</v>
@@ -1506,7 +1513,7 @@
         <v>0000101000100000000000000</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1514,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>128</v>
@@ -1586,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>129</v>
@@ -1650,7 +1657,7 @@
         <v>0000000000000000111100000</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -1658,7 +1665,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>130</v>
@@ -1722,7 +1729,7 @@
         <v>0000000101000000000000000</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1730,7 +1737,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>131</v>
@@ -1802,7 +1809,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>132</v>
@@ -1866,7 +1873,7 @@
         <v xml:space="preserve">0000000101000111000000001 </v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1874,7 +1881,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>133</v>
@@ -1904,10 +1911,10 @@
         <v>124</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>127</v>
@@ -1933,12 +1940,12 @@
       <c r="U8" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="V8" s="4" t="str">
+      <c r="V8" s="6" t="str">
         <f>E8&amp;F8&amp;G8&amp;H8&amp;I8&amp;J8&amp;K8&amp;L8&amp;M8&amp;N8&amp;O8&amp;P8&amp;Q8&amp;R8&amp;S8&amp;T8&amp;U8</f>
-        <v>0000101101000111000000001</v>
+        <v>0000101101111111000000001</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>204</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -1946,7 +1953,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>134</v>
@@ -2010,7 +2017,7 @@
         <v>0000000000000000001100001</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -2018,7 +2025,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>135</v>
@@ -2090,7 +2097,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>136</v>
@@ -2154,7 +2161,7 @@
         <v>0000000111000000000000000</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -2162,7 +2169,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>137</v>
@@ -2226,7 +2233,7 @@
         <v>0000000110000000000000000</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -2234,7 +2241,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>138</v>
@@ -2298,7 +2305,7 @@
         <v>0000101000111000110000100</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -2306,7 +2313,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>139</v>
@@ -2370,7 +2377,7 @@
         <v>0000101000111000000000100</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -2378,7 +2385,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>140</v>
@@ -2442,7 +2449,7 @@
         <v>0000101000111000000000100</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2450,7 +2457,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>141</v>
@@ -2514,7 +2521,7 @@
         <v>0000000101000111110000100</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -2522,7 +2529,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>142</v>
@@ -2586,7 +2593,7 @@
         <v>0000000101000111000000100</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -2594,7 +2601,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>143</v>
@@ -2658,7 +2665,7 @@
         <v>0000000000000000000000100</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -2666,7 +2673,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>144</v>
@@ -2730,7 +2737,7 @@
         <v>0000101000111000110000110</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -2738,7 +2745,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>145</v>
@@ -2802,7 +2809,7 @@
         <v>0000000101000000110000110</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -2810,7 +2817,7 @@
         <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>146</v>
@@ -2874,7 +2881,7 @@
         <v>0000101000111000000000110</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -2882,7 +2889,7 @@
         <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>147</v>
@@ -2946,7 +2953,7 @@
         <v>0000000101000000000000110</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2954,7 +2961,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>148</v>
@@ -3018,7 +3025,7 @@
         <v>0000101000111000110000111</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -3026,7 +3033,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>149</v>
@@ -3090,7 +3097,7 @@
         <v>0000000101000111110000111</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -3098,7 +3105,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>150</v>
@@ -3162,7 +3169,7 @@
         <v>0000101000111000000000111</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -3170,7 +3177,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>151</v>
@@ -3234,7 +3241,7 @@
         <v>0000000101000111000000111</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -3242,7 +3249,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>152</v>
@@ -3306,7 +3313,7 @@
         <v>0000101000111000000000111</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
@@ -3314,7 +3321,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>153</v>
@@ -3378,7 +3385,7 @@
         <v>0000000101000111000000111</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
@@ -3386,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>154</v>
@@ -3450,7 +3457,7 @@
         <v>0000101000111000110001000</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -3458,7 +3465,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>155</v>
@@ -3522,7 +3529,7 @@
         <v>0000000101000111110001000</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -3530,7 +3537,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>156</v>
@@ -3594,7 +3601,7 @@
         <v>0000101000111000000001000</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
@@ -3602,7 +3609,7 @@
         <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>157</v>
@@ -3666,7 +3673,7 @@
         <v>0000000101000111000001000</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -3674,7 +3681,7 @@
         <v>41</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>158</v>
@@ -3738,7 +3745,7 @@
         <v>0000101000111000000001000</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -3746,7 +3753,7 @@
         <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>159</v>
@@ -3810,7 +3817,7 @@
         <v>0000000101000111000001000</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -3818,7 +3825,7 @@
         <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>160</v>
@@ -3882,7 +3889,7 @@
         <v>0000101000111000110000010</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -3890,7 +3897,7 @@
         <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>161</v>
@@ -3954,7 +3961,7 @@
         <v>0000000110000111110000010</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -3962,7 +3969,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>162</v>
@@ -4026,7 +4033,7 @@
         <v>0000101000111000000000010</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -4034,7 +4041,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>163</v>
@@ -4098,7 +4105,7 @@
         <v>0000000101000111000000010</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -4106,7 +4113,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>164</v>
@@ -4170,7 +4177,7 @@
         <v>0000101000111000110001010</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -4178,7 +4185,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>165</v>
@@ -4242,7 +4249,7 @@
         <v>0000000101000111110001010</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
@@ -4250,7 +4257,7 @@
         <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>166</v>
@@ -4314,7 +4321,7 @@
         <v>0000101000111000000001010</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
@@ -4322,7 +4329,7 @@
         <v>32</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>167</v>
@@ -4386,7 +4393,7 @@
         <v>0000000101000111000001010</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
@@ -4394,7 +4401,7 @@
         <v>31</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>168</v>
@@ -4458,7 +4465,7 @@
         <v>0000000101111000110001011</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -4466,7 +4473,7 @@
         <v>30</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>169</v>
@@ -4530,7 +4537,7 @@
         <v>0000000101000111000001011</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
@@ -4538,7 +4545,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>170</v>
@@ -4602,7 +4609,7 @@
         <v>0000101000111000000001011</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
@@ -4610,7 +4617,7 @@
         <v>28</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>171</v>
@@ -4674,7 +4681,7 @@
         <v>0000000101000111000001011</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
@@ -4682,7 +4689,7 @@
         <v>27</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>172</v>
@@ -4746,7 +4753,7 @@
         <v>0000000101000101000000000</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -4754,7 +4761,7 @@
         <v>26</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>173</v>
@@ -4818,7 +4825,7 @@
         <v>0000000000000000001100000</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
@@ -4826,7 +4833,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>174</v>
@@ -4890,7 +4897,7 @@
         <v>0000000101000110001010000</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
@@ -4898,7 +4905,7 @@
         <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>175</v>
@@ -4962,7 +4969,7 @@
         <v>0000000000000000000000000</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
@@ -4970,7 +4977,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>176</v>
@@ -5034,7 +5041,7 @@
         <v>0000000000000000110000000</v>
       </c>
       <c r="W51" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -5042,7 +5049,7 @@
         <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>177</v>
@@ -5106,7 +5113,7 @@
         <v>0000000111000000000000000</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
@@ -5114,7 +5121,7 @@
         <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>178</v>
@@ -5178,7 +5185,7 @@
         <v>0000111000000000000000000</v>
       </c>
       <c r="W53" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
@@ -5186,7 +5193,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>179</v>
@@ -5250,7 +5257,7 @@
         <v>0000000110000000000000000</v>
       </c>
       <c r="W54" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
@@ -5258,7 +5265,7 @@
         <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>180</v>
@@ -5322,7 +5329,7 @@
         <v>0000110000000000000000000</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
@@ -5330,7 +5337,7 @@
         <v>52</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>181</v>
@@ -5394,7 +5401,7 @@
         <v>1111000000000000001010000</v>
       </c>
       <c r="W56" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
@@ -5402,7 +5409,7 @@
         <v>53</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>182</v>
@@ -5466,7 +5473,7 @@
         <v>1110000000000000001010000</v>
       </c>
       <c r="W57" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
@@ -5474,7 +5481,7 @@
         <v>54</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>188</v>
@@ -5538,7 +5545,7 @@
         <v>0000000110000000000000000</v>
       </c>
       <c r="W58" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>